<commit_message>
fixed the mgr comment box id issue
</commit_message>
<xml_diff>
--- a/DataFolder/IPPB_EMP_Details.xlsx
+++ b/DataFolder/IPPB_EMP_Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\USRLocalization\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42D9856-BD73-48E1-8B0B-3051FB59E10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CDC44E-6228-4FEB-A121-94EA45BED583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Empoyee name</t>
   </si>
@@ -33,17 +33,308 @@
     <t>PMS Goal Plan Name</t>
   </si>
   <si>
-    <t>manuc@gmail.com</t>
-  </si>
-  <si>
-    <t>ajantha@usrinfotech.com</t>
+    <t>kanav.kapoor@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sashikant.panda@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sunil.sasegh@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>giriraj.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>easwaran.v@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>r.viswesvaran@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>neeraj.kj@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>jvenkatramu@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>maanus.cg@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sana.ps@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>satyabrata.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sailesh.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>tushar.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>poulomi.b@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>asheet.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>gautam.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>chikkala.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>lokesh.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sandeep.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>satyam.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shankar.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ankur.bhatt@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>makarand.ac@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pankaj.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sunny.db@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>nishant.c@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sunil.kr@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>deepika.u@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>greeshma.ur@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>prashant.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>himanshu.v@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>hemant.l@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>rajender.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pradeep.kn@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ANANDA.SWAROOP@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sandip.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>karrebatthula.n@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>mukund.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>mukul.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>Priyanka.bhatnagar@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>amit.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ranveer.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shailesh.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>debarpan.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>manish.t@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>alkesh.y@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>anjali.r@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>amit.agrawal@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>anju.g@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>priyank.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>nikhil.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>mohankumar.n@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>poosarla.vs@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>Prashant.ds@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shailendra.t@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>RAJENDRA.P@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sumit.b@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ch.shobha@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>dhiren.mb@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>manoj.kv@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sajjan.g@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>jaipal@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sriram.b@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>yashodhi.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shubham.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>santosh.km@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>RR.KARTHIKEYAN@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>abhirup.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>vivek.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>meenakshi.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>nitase.bp@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>daseesh.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>karthick@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sampath.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shraddha.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>magesh.v@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>prateek.ma@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>vijay.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>guduru.nd@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>santosh.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ikbal.ps@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sachase.kadam@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pradeep.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>satyajit.t@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>arunkumar.r@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>vaseoth.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>rishabh.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>amit.ku@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sarthak.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>rajiv.kd@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>kiran.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>atul.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shashi.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>vikas.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>MANOHAR.l@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pankaj.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>anupam.c@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>regal.scr@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>masegma.s@cupoffline.ase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +345,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,16 +386,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +772,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2">
@@ -458,14 +780,793 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>123</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1A79517A-79E2-4D8E-84E6-4B280FBF72BC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added video pop-up close
</commit_message>
<xml_diff>
--- a/DataFolder/IPPB_EMP_Details.xlsx
+++ b/DataFolder/IPPB_EMP_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\USRLocalization\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C6E744-0B5B-4082-A8DC-509013EEFF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F028976-76F1-4D2D-A2D0-839043476AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Empoyee name</t>
   </si>
@@ -33,6 +33,261 @@
     <t>PMS Goal Plan Name</t>
   </si>
   <si>
+    <t>rishabh.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>amit.ku@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sarthak.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>rajiv.kd@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>kiran.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>atul.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shashi.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>vikas.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>MANOHAR.l@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pankaj.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>anupam.c@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>regal.scr@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>masegma.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>kanav.kapoor@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sashikant.panda@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sunil.sasegh@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>giriraj.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>easwaran.v@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>r.viswesvaran@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>neeraj.kj@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>jvenkatramu@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>maanus.cg@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sana.ps@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>satyabrata.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sailesh.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>tushar.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>poulomi.b@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>asheet.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>gautam.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>chikkala.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>lokesh.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sandeep.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>satyam.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shankar.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ankur.bhatt@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>makarand.ac@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pankaj.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sunny.db@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>nishant.c@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sunil.kr@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>deepika.u@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>greeshma.ur@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>prashant.ks@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>himanshu.v@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>hemant.l@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>rajender.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>pradeep.kn@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ANANDA.SWAROOP@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sandip.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>karrebatthula.n@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>mukund.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>mukul.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>Priyanka.bhatnagar@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>amit.k@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ranveer.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shailesh.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>debarpan.d@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>manish.t@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>alkesh.y@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>anjali.r@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>amit.agrawal@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>anju.g@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>priyank.a@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>nikhil.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>mohankumar.n@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>poosarla.vs@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>Prashant.ds@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shailendra.t@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>RAJENDRA.P@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sumit.b@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>ch.shobha@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>dhiren.mb@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>manoj.kv@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sajjan.g@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>jaipal@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>sriram.b@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>yashodhi.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>shubham.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>santosh.km@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>RR.KARTHIKEYAN@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>abhirup.p@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>vivek.s@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>meenakshi.m@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>nitase.bp@cupoffline.ase</t>
+  </si>
+  <si>
+    <t>daseesh.k@cupoffline.ase</t>
+  </si>
+  <si>
     <t>karthick@cupoffline.ase</t>
   </si>
   <si>
@@ -73,265 +328,13 @@
   </si>
   <si>
     <t>vaseoth.ks@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>rishabh.k@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>amit.ku@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sarthak.m@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>rajiv.kd@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>kiran.d@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>atul.k@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>shashi.p@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>vikas.a@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>MANOHAR.l@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>pankaj.d@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>anupam.c@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>regal.scr@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>masegma.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sashikant.panda@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sunil.sasegh@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>giriraj.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>easwaran.v@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>r.viswesvaran@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>neeraj.kj@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>jvenkatramu@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>maanus.cg@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sana.ps@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>satyabrata.p@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sailesh.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>tushar.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>poulomi.b@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>asheet.a@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>gautam.m@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>chikkala.a@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>lokesh.k@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sandeep.ks@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>satyam.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>shankar.p@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>ankur.bhatt@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>makarand.ac@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>pankaj.ks@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sunny.db@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>nishant.c@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sunil.kr@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>deepika.u@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>greeshma.ur@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>prashant.ks@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>himanshu.v@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>hemant.l@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>rajender.m@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>pradeep.kn@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>ANANDA.SWAROOP@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sandip.k@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>karrebatthula.n@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>mukund.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>mukul.a@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>Priyanka.bhatnagar@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>amit.k@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>ranveer.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>shailesh.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>debarpan.d@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>manish.t@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>alkesh.y@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>anjali.r@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>amit.agrawal@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>anju.g@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>priyank.a@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>nikhil.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>mohankumar.n@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>poosarla.vs@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>Prashant.ds@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>shailendra.t@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>RAJENDRA.P@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sumit.b@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>ch.shobha@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>dhiren.mb@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>manoj.kv@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sajjan.g@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>jaipal@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>sriram.b@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>yashodhi.p@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>shubham.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>santosh.km@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>RR.KARTHIKEYAN@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>abhirup.p@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>vivek.s@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>meenakshi.m@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>nitase.bp@cupoffline.ase</t>
-  </si>
-  <si>
-    <t>daseesh.k@cupoffline.ase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +354,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -397,18 +408,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,8 +778,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
+      <c r="A2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B2">
         <v>123</v>
@@ -771,7 +787,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>123</v>
@@ -779,7 +795,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>123</v>
@@ -787,7 +803,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>123</v>
@@ -795,7 +811,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>123</v>
@@ -803,7 +819,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>123</v>
@@ -811,7 +827,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>123</v>
@@ -819,7 +835,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>123</v>
@@ -827,7 +843,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>123</v>
@@ -835,7 +851,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>123</v>
@@ -843,7 +859,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>123</v>
@@ -851,7 +867,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>123</v>
@@ -859,7 +875,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>123</v>
@@ -867,7 +883,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>123</v>
@@ -875,7 +891,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>123</v>
@@ -883,7 +899,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>123</v>
@@ -891,7 +907,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>123</v>
@@ -899,7 +915,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>123</v>
@@ -907,7 +923,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>123</v>
@@ -915,7 +931,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>123</v>
@@ -923,7 +939,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B22">
         <v>123</v>
@@ -931,7 +947,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>123</v>
@@ -939,7 +955,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>123</v>
@@ -947,7 +963,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>123</v>
@@ -955,7 +971,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>123</v>
@@ -963,7 +979,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B27">
         <v>123</v>
@@ -971,7 +987,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>123</v>
@@ -979,7 +995,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B29">
         <v>123</v>
@@ -987,7 +1003,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>123</v>
@@ -995,7 +1011,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>123</v>
@@ -1003,7 +1019,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>123</v>
@@ -1011,7 +1027,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B33">
         <v>123</v>
@@ -1019,7 +1035,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B34">
         <v>123</v>
@@ -1027,7 +1043,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>123</v>
@@ -1035,7 +1051,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B36">
         <v>123</v>
@@ -1043,7 +1059,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B37">
         <v>123</v>
@@ -1051,7 +1067,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B38">
         <v>123</v>
@@ -1059,7 +1075,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B39">
         <v>123</v>
@@ -1067,7 +1083,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B40">
         <v>123</v>
@@ -1075,7 +1091,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B41">
         <v>123</v>
@@ -1083,7 +1099,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B42">
         <v>123</v>
@@ -1091,7 +1107,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B43">
         <v>123</v>
@@ -1099,7 +1115,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B44">
         <v>123</v>
@@ -1107,7 +1123,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B45">
         <v>123</v>
@@ -1115,7 +1131,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B46">
         <v>123</v>
@@ -1123,7 +1139,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B47">
         <v>123</v>
@@ -1131,7 +1147,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B48">
         <v>123</v>
@@ -1139,7 +1155,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B49">
         <v>123</v>
@@ -1147,7 +1163,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B50">
         <v>123</v>
@@ -1155,7 +1171,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B51">
         <v>123</v>
@@ -1163,7 +1179,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B52">
         <v>123</v>
@@ -1171,7 +1187,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B53">
         <v>123</v>
@@ -1179,7 +1195,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B54">
         <v>123</v>
@@ -1187,7 +1203,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B55">
         <v>123</v>
@@ -1195,7 +1211,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B56">
         <v>123</v>
@@ -1203,7 +1219,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B57">
         <v>123</v>
@@ -1211,7 +1227,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B58">
         <v>123</v>
@@ -1219,7 +1235,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>123</v>
@@ -1227,7 +1243,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B60">
         <v>123</v>
@@ -1235,7 +1251,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B61">
         <v>123</v>
@@ -1243,7 +1259,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B62">
         <v>123</v>
@@ -1251,7 +1267,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B63">
         <v>123</v>
@@ -1259,7 +1275,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B64">
         <v>123</v>
@@ -1267,7 +1283,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B65">
         <v>123</v>
@@ -1275,7 +1291,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B66">
         <v>123</v>
@@ -1283,7 +1299,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B67">
         <v>123</v>
@@ -1291,7 +1307,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B68">
         <v>123</v>
@@ -1299,7 +1315,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B69">
         <v>123</v>
@@ -1307,7 +1323,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B70">
         <v>123</v>
@@ -1315,7 +1331,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B71">
         <v>123</v>
@@ -1323,7 +1339,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B72">
         <v>123</v>
@@ -1331,7 +1347,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B73">
         <v>123</v>
@@ -1339,7 +1355,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B74">
         <v>123</v>
@@ -1347,7 +1363,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="B75">
         <v>123</v>
@@ -1355,7 +1371,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="B76">
         <v>123</v>
@@ -1363,7 +1379,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="B77">
         <v>123</v>
@@ -1371,7 +1387,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="B78">
         <v>123</v>
@@ -1379,7 +1395,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="B79">
         <v>123</v>
@@ -1387,7 +1403,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="B80">
         <v>123</v>
@@ -1395,7 +1411,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="B81">
         <v>123</v>
@@ -1403,7 +1419,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B82">
         <v>123</v>
@@ -1411,7 +1427,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="B83">
         <v>123</v>
@@ -1419,7 +1435,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="B84">
         <v>123</v>
@@ -1427,7 +1443,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="B85">
         <v>123</v>
@@ -1435,7 +1451,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B86">
         <v>123</v>
@@ -1443,7 +1459,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B87">
         <v>123</v>
@@ -1451,7 +1467,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B88">
         <v>123</v>
@@ -1459,7 +1475,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B89">
         <v>123</v>
@@ -1467,7 +1483,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B90">
         <v>123</v>
@@ -1475,7 +1491,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B91">
         <v>123</v>
@@ -1483,7 +1499,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B92">
         <v>123</v>
@@ -1491,7 +1507,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B93">
         <v>123</v>
@@ -1499,7 +1515,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B94">
         <v>123</v>
@@ -1507,7 +1523,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B95">
         <v>123</v>
@@ -1515,7 +1531,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B96">
         <v>123</v>
@@ -1523,7 +1539,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B97">
         <v>123</v>
@@ -1531,7 +1547,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B98">
         <v>123</v>
@@ -1539,13 +1555,24 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B99">
         <v>123</v>
       </c>
     </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:kanav.kapoor@cupoffline.ase" xr:uid="{CD76942F-B2E2-47AD-BB33-8D02EC664419}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed pop-up issue in all pages and some other issue
</commit_message>
<xml_diff>
--- a/DataFolder/IPPB_EMP_Details.xlsx
+++ b/DataFolder/IPPB_EMP_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\USRLocalization\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F028976-76F1-4D2D-A2D0-839043476AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41042E0-9EDB-45E6-9D1F-57164ED1FCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>